<commit_message>
Seed file updated. But it has errors
</commit_message>
<xml_diff>
--- a/db/kocgiri01.xlsx
+++ b/db/kocgiri01.xlsx
@@ -208,7 +208,7 @@
     <t xml:space="preserve">17.3.1337</t>
   </si>
   <si>
-    <t xml:space="preserve">Elazığ Vali Vekili Abdülkadir, Erzincan mutasarrıfı Ali Rıza, Merkez Ordusu Kumandan-ı Sani Erkan-ı Harbiye Reisi Hüseyin Hüsnü, Mevki Kumandanı Baki, 14. Fırka Kumandanı Hayri, </t>
+    <t xml:space="preserve">Elazığ Vali Vekili Abdülkadir, Erzincan Mutasarrıfı Ali Rıza, Merkez Ordusu Kumandan-ı Sani Erkan-ı Harbiye Reisi Hüseyin Hüsnü, Mevki Kumandanı Baki, 14. Fırka Kumandanı Hayri, </t>
   </si>
   <si>
     <t xml:space="preserve">Tokad Ordu Kumandanlığı, Erzincan Mevki Kumandanlığı, Erzincan Mutasarrıflığı, </t>
@@ -238,7 +238,7 @@
     <t xml:space="preserve">19.3.1337</t>
   </si>
   <si>
-    <t xml:space="preserve">Merkez Ordusu Kumandanı Nurettin, Nurettin Paşa, Merkez Ordusu Kumandanı Nurettin İbrahim Sakallı Nurettin, Merkez Ordusu Kumandanı Nureddin, Nureddin Paşa, Merkez Ordusu Kumandanı Nureddin İbrahim, Sakallı Nureddin, Sivas Valisi Cemal, Erkan-ı Harbiye Umumiye Reisi Hüseyin Hüsnü,  Giresun Alay-ı Fahri Kumandanı Osman, Erzincan Mutasarrıfı Ali Rıza, Erzincan Mevki kumandanı Baki, Mustafpaşazade Hayri, Alişenbeyzade Mahmud, Timurağazade Ali, Karaeyübzade Rıza, Sadattan Topuzluzade İbrahim</t>
+    <t xml:space="preserve">Merkez Ordusu Kumandanı Nurettin, Nurettin Paşa, Merkez Ordusu Kumandanı Nurettin İbrahim Sakallı Nurettin, Merkez Ordusu Kumandanı Nureddin, Nureddin Paşa, Merkez Ordusu Kumandanı Nureddin İbrahim, Sakallı Nureddin, Sivas Valisi Cemal, Erkan-ı Harbiye Umumiye Reisi Hüseyin Hüsnü,  Giresun Alay-ı Fahri Kumandanı Osman, Erzincan Mutasarrıfı Ali Rıza, Erzincan Mevki Kumandanı Baki, Mustafpaşazade Hayri, Alişenbeyzade Mahmud, Timurağazade Ali, Karaeyübzade Rıza, Sadattan Topuzluzade İbrahim</t>
   </si>
   <si>
     <t xml:space="preserve">Merkez Ordusu Kumandanlığı, Erzincan Mevki kumandanlığı, Erkan-ı Harbiye Umumi Riyaseti, Müdafa-ı Milliye Vekaleti, Şark Cephesi Kumandanlığı, Elcezire Cephesi Kumandanılığı, 2. Fırka Kumandanlığı, 14. Fırka Kumandanlığı, </t>
@@ -4190,10 +4190,10 @@
   </sheetPr>
   <dimension ref="A1:L260"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E81" activeCellId="0" sqref="E81"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>